<commit_message>
Dataset increased to 39
</commit_message>
<xml_diff>
--- a/dyes_DFT_PBE_eth_dataset.xlsx
+++ b/dyes_DFT_PBE_eth_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1394,340 +1394,408 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Phenothiazine1</t>
+          <t>MS-C</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-4.935</v>
+        <v>-4.722</v>
       </c>
       <c r="C29" t="n">
-        <v>-3.333</v>
+        <v>-3.386</v>
       </c>
       <c r="D29" t="n">
-        <v>9.0352</v>
+        <v>12.4976</v>
       </c>
       <c r="E29" t="n">
-        <v>-1351.57215</v>
+        <v>-2524.737106</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.765</v>
+        <v>-1.229</v>
       </c>
       <c r="G29" t="n">
-        <v>330.452395</v>
+        <v>664.014608</v>
       </c>
       <c r="H29" t="n">
-        <v>349.95115</v>
+        <v>750.022794</v>
       </c>
       <c r="I29" t="n">
-        <v>343</v>
+        <v>524</v>
       </c>
       <c r="J29" t="n">
-        <v>0.288586</v>
+        <v>0.540054</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Phenothiazine2</t>
+          <t>MS-M</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.818</v>
+        <v>-4.847</v>
       </c>
       <c r="C30" t="n">
-        <v>-2.806</v>
+        <v>-3.416</v>
       </c>
       <c r="D30" t="n">
-        <v>7.2013</v>
+        <v>13.6713</v>
       </c>
       <c r="E30" t="n">
-        <v>-1259.394134</v>
+        <v>-1891.093586</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.631</v>
+        <v>-0.948</v>
       </c>
       <c r="G30" t="n">
-        <v>311.25871</v>
+        <v>461.204862</v>
       </c>
       <c r="H30" t="n">
-        <v>327.396927</v>
+        <v>518.497894</v>
       </c>
       <c r="I30" t="n">
-        <v>308</v>
+        <v>664</v>
       </c>
       <c r="J30" t="n">
-        <v>0.353802</v>
+        <v>0.313744</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Phenothiazine3</t>
+          <t>Phenothiazine1</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-5.34</v>
+        <v>-4.935</v>
       </c>
       <c r="C31" t="n">
-        <v>-3.153</v>
+        <v>-3.333</v>
       </c>
       <c r="D31" t="n">
-        <v>9.789300000000001</v>
+        <v>9.0352</v>
       </c>
       <c r="E31" t="n">
-        <v>-953.539237</v>
+        <v>-1351.57215</v>
       </c>
       <c r="F31" t="n">
         <v>-0.765</v>
       </c>
       <c r="G31" t="n">
-        <v>310.115745</v>
+        <v>330.452395</v>
       </c>
       <c r="H31" t="n">
-        <v>326.248824</v>
+        <v>349.95115</v>
       </c>
       <c r="I31" t="n">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="J31" t="n">
-        <v>0.479784</v>
+        <v>0.288586</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Phenothiazine4</t>
+          <t>Phenothiazine2</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-4.991</v>
+        <v>-4.818</v>
       </c>
       <c r="C32" t="n">
-        <v>-3.206</v>
+        <v>-2.806</v>
       </c>
       <c r="D32" t="n">
-        <v>9.4053</v>
+        <v>7.2013</v>
       </c>
       <c r="E32" t="n">
-        <v>-1032.044192</v>
+        <v>-1259.394134</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.759</v>
+        <v>-0.631</v>
       </c>
       <c r="G32" t="n">
-        <v>333.827291</v>
+        <v>311.25871</v>
       </c>
       <c r="H32" t="n">
-        <v>358.719796</v>
+        <v>327.396927</v>
       </c>
       <c r="I32" t="n">
-        <v>524</v>
+        <v>308</v>
       </c>
       <c r="J32" t="n">
-        <v>0.534846</v>
+        <v>0.353802</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Quercitin</t>
+          <t>Phenothiazine3</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-5.323</v>
+        <v>-5.34</v>
       </c>
       <c r="C33" t="n">
-        <v>-2.754</v>
+        <v>-3.153</v>
       </c>
       <c r="D33" t="n">
-        <v>6.6676</v>
+        <v>9.789300000000001</v>
       </c>
       <c r="E33" t="n">
-        <v>-1638.590312</v>
+        <v>-953.539237</v>
       </c>
       <c r="F33" t="n">
-        <v>-1.058</v>
+        <v>-0.765</v>
       </c>
       <c r="G33" t="n">
-        <v>381.893317</v>
+        <v>310.115745</v>
       </c>
       <c r="H33" t="n">
-        <v>426.986904</v>
+        <v>326.248824</v>
       </c>
       <c r="I33" t="n">
-        <v>419</v>
+        <v>332</v>
       </c>
       <c r="J33" t="n">
-        <v>0.193758</v>
+        <v>0.479784</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Rutin</t>
+          <t>Phenothiazine4</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-5.159</v>
+        <v>-4.991</v>
       </c>
       <c r="C34" t="n">
-        <v>-2.833</v>
+        <v>-3.206</v>
       </c>
       <c r="D34" t="n">
-        <v>6.3594</v>
+        <v>9.4053</v>
       </c>
       <c r="E34" t="n">
-        <v>-2710.037461</v>
+        <v>-1032.044192</v>
       </c>
       <c r="F34" t="n">
-        <v>-1.971</v>
+        <v>-0.759</v>
       </c>
       <c r="G34" t="n">
-        <v>631.881213</v>
+        <v>333.827291</v>
       </c>
       <c r="H34" t="n">
-        <v>731.916619</v>
+        <v>358.719796</v>
       </c>
       <c r="I34" t="n">
-        <v>466</v>
+        <v>524</v>
       </c>
       <c r="J34" t="n">
-        <v>0.255696</v>
+        <v>0.534846</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>Quercitin</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-5.418</v>
+        <v>-5.323</v>
       </c>
       <c r="C35" t="n">
-        <v>-3.71</v>
+        <v>-2.754</v>
       </c>
       <c r="D35" t="n">
-        <v>14.832</v>
+        <v>6.6676</v>
       </c>
       <c r="E35" t="n">
-        <v>-1464.797419</v>
+        <v>-1638.590312</v>
       </c>
       <c r="F35" t="n">
-        <v>-1.012</v>
+        <v>-1.058</v>
       </c>
       <c r="G35" t="n">
-        <v>373.33181</v>
+        <v>381.893317</v>
       </c>
       <c r="H35" t="n">
-        <v>386.599372</v>
+        <v>426.986904</v>
       </c>
       <c r="I35" t="n">
-        <v>523</v>
+        <v>419</v>
       </c>
       <c r="J35" t="n">
-        <v>0.952597</v>
+        <v>0.193758</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>Rutin</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-5.396</v>
+        <v>-5.159</v>
       </c>
       <c r="C36" t="n">
-        <v>-3.71</v>
+        <v>-2.833</v>
       </c>
       <c r="D36" t="n">
-        <v>15.8432</v>
+        <v>6.3594</v>
       </c>
       <c r="E36" t="n">
-        <v>-1618.511711</v>
+        <v>-2710.037461</v>
       </c>
       <c r="F36" t="n">
-        <v>-1.097</v>
+        <v>-1.971</v>
       </c>
       <c r="G36" t="n">
-        <v>417.523898</v>
+        <v>631.881213</v>
       </c>
       <c r="H36" t="n">
-        <v>431.785193</v>
+        <v>731.916619</v>
       </c>
       <c r="I36" t="n">
-        <v>540</v>
+        <v>466</v>
       </c>
       <c r="J36" t="n">
-        <v>0.7944870000000001</v>
+        <v>0.255696</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-5.448</v>
+        <v>-5.418</v>
       </c>
       <c r="C37" t="n">
-        <v>-3.863</v>
+        <v>-3.71</v>
       </c>
       <c r="D37" t="n">
-        <v>13.091</v>
+        <v>14.832</v>
       </c>
       <c r="E37" t="n">
-        <v>-1633.444146</v>
+        <v>-1464.797419</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.952</v>
+        <v>-1.012</v>
       </c>
       <c r="G37" t="n">
-        <v>393.928755</v>
+        <v>373.33181</v>
       </c>
       <c r="H37" t="n">
-        <v>413.254515</v>
+        <v>386.599372</v>
       </c>
       <c r="I37" t="n">
-        <v>560</v>
+        <v>523</v>
       </c>
       <c r="J37" t="n">
-        <v>1.005572</v>
+        <v>0.952597</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>-5.396</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-3.71</v>
+      </c>
+      <c r="D38" t="n">
+        <v>15.8432</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-1618.511711</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-1.097</v>
+      </c>
+      <c r="G38" t="n">
+        <v>417.523898</v>
+      </c>
+      <c r="H38" t="n">
+        <v>431.785193</v>
+      </c>
+      <c r="I38" t="n">
+        <v>540</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.7944870000000001</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>-5.448</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-3.863</v>
+      </c>
+      <c r="D39" t="n">
+        <v>13.091</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-1633.444146</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.952</v>
+      </c>
+      <c r="G39" t="n">
+        <v>393.928755</v>
+      </c>
+      <c r="H39" t="n">
+        <v>413.254515</v>
+      </c>
+      <c r="I39" t="n">
+        <v>560</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1.005572</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>T4</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B40" t="n">
         <v>-5.429</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C40" t="n">
         <v>-3.866</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D40" t="n">
         <v>13.7502</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E40" t="n">
         <v>-1787.160542</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F40" t="n">
         <v>-1.021</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G40" t="n">
         <v>441.173419</v>
       </c>
-      <c r="H38" t="n">
+      <c r="H40" t="n">
         <v>457.649836</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I40" t="n">
         <v>583</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J40" t="n">
         <v>0.7942709999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed PCA and Enhanced plots, increased dataset to 40.
</commit_message>
<xml_diff>
--- a/dyes_DFT_PBE_eth_dataset.xlsx
+++ b/dyes_DFT_PBE_eth_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1428,374 +1428,408 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MS-M</t>
+          <t>MS-F</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-4.847</v>
+        <v>-4.86</v>
       </c>
       <c r="C30" t="n">
-        <v>-3.416</v>
+        <v>-3.442</v>
       </c>
       <c r="D30" t="n">
-        <v>13.6713</v>
+        <v>13.288</v>
       </c>
       <c r="E30" t="n">
-        <v>-1891.093586</v>
+        <v>-2665.761431</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.948</v>
+        <v>-1.129</v>
       </c>
       <c r="G30" t="n">
-        <v>461.204862</v>
+        <v>727.90863</v>
       </c>
       <c r="H30" t="n">
-        <v>518.497894</v>
+        <v>831.593118</v>
       </c>
       <c r="I30" t="n">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="J30" t="n">
-        <v>0.313744</v>
+        <v>0.321307</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Phenothiazine1</t>
+          <t>MS-M</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-4.935</v>
+        <v>-4.847</v>
       </c>
       <c r="C31" t="n">
-        <v>-3.333</v>
+        <v>-3.416</v>
       </c>
       <c r="D31" t="n">
-        <v>9.0352</v>
+        <v>13.6713</v>
       </c>
       <c r="E31" t="n">
-        <v>-1351.57215</v>
+        <v>-1891.093586</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.765</v>
+        <v>-0.948</v>
       </c>
       <c r="G31" t="n">
-        <v>330.452395</v>
+        <v>461.204862</v>
       </c>
       <c r="H31" t="n">
-        <v>349.95115</v>
+        <v>518.497894</v>
       </c>
       <c r="I31" t="n">
-        <v>343</v>
+        <v>664</v>
       </c>
       <c r="J31" t="n">
-        <v>0.288586</v>
+        <v>0.313744</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Phenothiazine2</t>
+          <t>Phenothiazine1</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-4.818</v>
+        <v>-4.935</v>
       </c>
       <c r="C32" t="n">
-        <v>-2.806</v>
+        <v>-3.333</v>
       </c>
       <c r="D32" t="n">
-        <v>7.2013</v>
+        <v>9.0352</v>
       </c>
       <c r="E32" t="n">
-        <v>-1259.394134</v>
+        <v>-1351.57215</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.631</v>
+        <v>-0.765</v>
       </c>
       <c r="G32" t="n">
-        <v>311.25871</v>
+        <v>330.452395</v>
       </c>
       <c r="H32" t="n">
-        <v>327.396927</v>
+        <v>349.95115</v>
       </c>
       <c r="I32" t="n">
-        <v>308</v>
+        <v>343</v>
       </c>
       <c r="J32" t="n">
-        <v>0.353802</v>
+        <v>0.288586</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Phenothiazine3</t>
+          <t>Phenothiazine2</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-5.34</v>
+        <v>-4.818</v>
       </c>
       <c r="C33" t="n">
-        <v>-3.153</v>
+        <v>-2.806</v>
       </c>
       <c r="D33" t="n">
-        <v>9.789300000000001</v>
+        <v>7.2013</v>
       </c>
       <c r="E33" t="n">
-        <v>-953.539237</v>
+        <v>-1259.394134</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.765</v>
+        <v>-0.631</v>
       </c>
       <c r="G33" t="n">
-        <v>310.115745</v>
+        <v>311.25871</v>
       </c>
       <c r="H33" t="n">
-        <v>326.248824</v>
+        <v>327.396927</v>
       </c>
       <c r="I33" t="n">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="J33" t="n">
-        <v>0.479784</v>
+        <v>0.353802</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Phenothiazine4</t>
+          <t>Phenothiazine3</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-4.991</v>
+        <v>-5.34</v>
       </c>
       <c r="C34" t="n">
-        <v>-3.206</v>
+        <v>-3.153</v>
       </c>
       <c r="D34" t="n">
-        <v>9.4053</v>
+        <v>9.789300000000001</v>
       </c>
       <c r="E34" t="n">
-        <v>-1032.044192</v>
+        <v>-953.539237</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.759</v>
+        <v>-0.765</v>
       </c>
       <c r="G34" t="n">
-        <v>333.827291</v>
+        <v>310.115745</v>
       </c>
       <c r="H34" t="n">
-        <v>358.719796</v>
+        <v>326.248824</v>
       </c>
       <c r="I34" t="n">
-        <v>524</v>
+        <v>332</v>
       </c>
       <c r="J34" t="n">
-        <v>0.534846</v>
+        <v>0.479784</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Quercitin</t>
+          <t>Phenothiazine4</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-5.323</v>
+        <v>-4.991</v>
       </c>
       <c r="C35" t="n">
-        <v>-2.754</v>
+        <v>-3.206</v>
       </c>
       <c r="D35" t="n">
-        <v>6.6676</v>
+        <v>9.4053</v>
       </c>
       <c r="E35" t="n">
-        <v>-1638.590312</v>
+        <v>-1032.044192</v>
       </c>
       <c r="F35" t="n">
-        <v>-1.058</v>
+        <v>-0.759</v>
       </c>
       <c r="G35" t="n">
-        <v>381.893317</v>
+        <v>333.827291</v>
       </c>
       <c r="H35" t="n">
-        <v>426.986904</v>
+        <v>358.719796</v>
       </c>
       <c r="I35" t="n">
-        <v>419</v>
+        <v>524</v>
       </c>
       <c r="J35" t="n">
-        <v>0.193758</v>
+        <v>0.534846</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Rutin</t>
+          <t>Quercitin</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-5.159</v>
+        <v>-5.323</v>
       </c>
       <c r="C36" t="n">
-        <v>-2.833</v>
+        <v>-2.754</v>
       </c>
       <c r="D36" t="n">
-        <v>6.3594</v>
+        <v>6.6676</v>
       </c>
       <c r="E36" t="n">
-        <v>-2710.037461</v>
+        <v>-1638.590312</v>
       </c>
       <c r="F36" t="n">
-        <v>-1.971</v>
+        <v>-1.058</v>
       </c>
       <c r="G36" t="n">
-        <v>631.881213</v>
+        <v>381.893317</v>
       </c>
       <c r="H36" t="n">
-        <v>731.916619</v>
+        <v>426.986904</v>
       </c>
       <c r="I36" t="n">
-        <v>466</v>
+        <v>419</v>
       </c>
       <c r="J36" t="n">
-        <v>0.255696</v>
+        <v>0.193758</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>Rutin</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-5.418</v>
+        <v>-5.159</v>
       </c>
       <c r="C37" t="n">
-        <v>-3.71</v>
+        <v>-2.833</v>
       </c>
       <c r="D37" t="n">
-        <v>14.832</v>
+        <v>6.3594</v>
       </c>
       <c r="E37" t="n">
-        <v>-1464.797419</v>
+        <v>-2710.037461</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.012</v>
+        <v>-1.971</v>
       </c>
       <c r="G37" t="n">
-        <v>373.33181</v>
+        <v>631.881213</v>
       </c>
       <c r="H37" t="n">
-        <v>386.599372</v>
+        <v>731.916619</v>
       </c>
       <c r="I37" t="n">
-        <v>523</v>
+        <v>466</v>
       </c>
       <c r="J37" t="n">
-        <v>0.952597</v>
+        <v>0.255696</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-5.396</v>
+        <v>-5.418</v>
       </c>
       <c r="C38" t="n">
         <v>-3.71</v>
       </c>
       <c r="D38" t="n">
-        <v>15.8432</v>
+        <v>14.832</v>
       </c>
       <c r="E38" t="n">
-        <v>-1618.511711</v>
+        <v>-1464.797419</v>
       </c>
       <c r="F38" t="n">
-        <v>-1.097</v>
+        <v>-1.012</v>
       </c>
       <c r="G38" t="n">
-        <v>417.523898</v>
+        <v>373.33181</v>
       </c>
       <c r="H38" t="n">
-        <v>431.785193</v>
+        <v>386.599372</v>
       </c>
       <c r="I38" t="n">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="J38" t="n">
-        <v>0.7944870000000001</v>
+        <v>0.952597</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-5.448</v>
+        <v>-5.396</v>
       </c>
       <c r="C39" t="n">
-        <v>-3.863</v>
+        <v>-3.71</v>
       </c>
       <c r="D39" t="n">
-        <v>13.091</v>
+        <v>15.8432</v>
       </c>
       <c r="E39" t="n">
-        <v>-1633.444146</v>
+        <v>-1618.511711</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.952</v>
+        <v>-1.097</v>
       </c>
       <c r="G39" t="n">
-        <v>393.928755</v>
+        <v>417.523898</v>
       </c>
       <c r="H39" t="n">
-        <v>413.254515</v>
+        <v>431.785193</v>
       </c>
       <c r="I39" t="n">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="J39" t="n">
-        <v>1.005572</v>
+        <v>0.7944870000000001</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>T3</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-5.448</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-3.863</v>
+      </c>
+      <c r="D40" t="n">
+        <v>13.091</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-1633.444146</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-0.952</v>
+      </c>
+      <c r="G40" t="n">
+        <v>393.928755</v>
+      </c>
+      <c r="H40" t="n">
+        <v>413.254515</v>
+      </c>
+      <c r="I40" t="n">
+        <v>560</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1.005572</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>T4</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B41" t="n">
         <v>-5.429</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C41" t="n">
         <v>-3.866</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D41" t="n">
         <v>13.7502</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E41" t="n">
         <v>-1787.160542</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F41" t="n">
         <v>-1.021</v>
       </c>
-      <c r="G40" t="n">
+      <c r="G41" t="n">
         <v>441.173419</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H41" t="n">
         <v>457.649836</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I41" t="n">
         <v>583</v>
       </c>
-      <c r="J40" t="n">
+      <c r="J41" t="n">
         <v>0.7942709999999999</v>
       </c>
     </row>

</xml_diff>